<commit_message>
Gestion dynamique des pages
En développement
</commit_message>
<xml_diff>
--- a/IMDD/Document/Planning_IMDD.xlsx
+++ b/IMDD/Document/Planning_IMDD.xlsx
@@ -16,12 +16,15 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$C$2:$I$22</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -63,6 +66,79 @@
   </si>
   <si>
     <t>Tests Unitaires</t>
+  </si>
+  <si>
+    <t>Projet IMDD</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Auteurs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Damjan, Dylan, Floran, Tom</t>
+    </r>
+  </si>
+  <si>
+    <t>Version 2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Date :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 16.03.2018</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -72,9 +148,25 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -95,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -254,11 +346,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -308,11 +473,177 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="29">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -350,186 +681,6 @@
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -873,385 +1024,429 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="C1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+    </row>
+    <row r="3" spans="3:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+    </row>
+    <row r="5" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="3:14" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="E6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F6" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="G6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="H6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="I6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19">
+      <c r="D7" s="19">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C2" s="24">
-        <f>SUM(D2:G2)</f>
+      <c r="E7" s="24">
+        <f>SUM(F7:I7)</f>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D2" s="6">
+      <c r="F7" s="6">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="E2" s="6">
+      <c r="G7" s="6">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="F2" s="6">
+      <c r="H7" s="6">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="G2" s="29">
+      <c r="I7" s="29">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="27"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="8" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17">
+      <c r="D9" s="17">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C4" s="24">
-        <f>SUM(D4:G4)</f>
+      <c r="E9" s="24">
+        <f t="shared" ref="E9:E14" si="0">SUM(F9:I9)</f>
+        <v>5.2083333333333329E-2</v>
+      </c>
+      <c r="F9" s="4">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="G9" s="7">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="30"/>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="30"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="17">
+      <c r="E10" s="24">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F10" s="4">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="17">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E11" s="24">
+        <f t="shared" si="0"/>
+        <v>5.2083333333333329E-2</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="I11" s="31"/>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="17">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E12" s="24">
+        <f t="shared" si="0"/>
+        <v>0.15625</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="H12" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="I12" s="31">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C5" s="24">
-        <f>SUM(D5:G5)</f>
+      <c r="M12" s="28"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="17">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E13" s="24">
+        <f t="shared" si="0"/>
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="F13" s="4">
         <v>3.125E-2</v>
       </c>
-      <c r="D5" s="4">
+      <c r="G13" s="4">
         <v>3.125E-2</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="17">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C6" s="24">
-        <f>SUM(D6:G6)</f>
-        <v>5.2083333333333329E-2</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="H13" s="4">
+        <v>3.125E-2</v>
+      </c>
+      <c r="I13" s="31">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F6" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="17">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C7" s="24">
-        <f>SUM(D7:G7)</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4">
-        <v>6.25E-2</v>
-      </c>
-      <c r="F7" s="4">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="L13" s="28"/>
+    </row>
+    <row r="14" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="K7" s="28"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="17">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C8" s="24">
-        <f>SUM(D8:G8)</f>
-        <v>0.11458333333333333</v>
-      </c>
-      <c r="D8" s="4">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E8" s="4">
-        <v>3.125E-2</v>
-      </c>
-      <c r="F8" s="4">
-        <v>3.125E-2</v>
-      </c>
-      <c r="G8" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="J8" s="28"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="17">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C9" s="24">
-        <f>SUM(D9:G9)</f>
+      <c r="E14" s="24">
+        <f t="shared" si="0"/>
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4">
+      <c r="F14" s="4"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="32">
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="27"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="20">
-        <f>SUM(B2:B10)</f>
+    <row r="15" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="12"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="27"/>
+    </row>
+    <row r="16" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="20">
+        <f t="shared" ref="D16:I16" si="1">SUM(D7:D15)</f>
         <v>0.52083333333333326</v>
       </c>
-      <c r="C11" s="26">
-        <f>SUM(C2:C10)</f>
+      <c r="E16" s="26">
+        <f t="shared" si="1"/>
         <v>0.49999999999999994</v>
       </c>
-      <c r="D11" s="22">
-        <f>SUM(D2:D10)</f>
+      <c r="F16" s="22">
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="E11" s="16">
-        <f>SUM(E2:E10)</f>
+      <c r="G16" s="16">
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="F11" s="16">
-        <f>SUM(F2:F10)</f>
+      <c r="H16" s="16">
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="G11" s="16">
-        <f>SUM(G2:G10)</f>
+      <c r="I16" s="16">
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H12" s="14">
-        <f>SUM(D11:G11)</f>
+    <row r="17" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I17" s="14">
+        <f>SUM(F16:I16)</f>
         <v>0.5</v>
       </c>
     </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="37"/>
+      <c r="H21" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="41"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="38"/>
+      <c r="D22" s="39"/>
+      <c r="H22" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="43"/>
+      <c r="J22" s="35"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:G2 D3:D10 F3:F10">
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:G2 D4:G9">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="greaterThan">
+  <mergeCells count="4">
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="C21:D22"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F7:I7 F8:F15 H8:H15">
+    <cfRule type="cellIs" dxfId="28" priority="34" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:I7 F9:I14">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3 D2:G10">
-    <cfRule type="cellIs" dxfId="32" priority="26" operator="greaterThan">
+  <conditionalFormatting sqref="E8 F7:I15">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="28" priority="23" operator="greaterThan">
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="25" priority="21" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="24" priority="20" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="21" priority="17" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
+  <conditionalFormatting sqref="I14">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>